<commit_message>
adds Python display functionality
</commit_message>
<xml_diff>
--- a/controlvars.xlsx
+++ b/controlvars.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnnyvenom/Documents/Projects/Noisebox-2018/iPad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnnyvenom/Documents/Projects/Noisebox-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD521DD-BCFC-6B4B-8926-36825823FC14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28A0197-1D7D-A348-95F6-F019930526DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9100" yWindow="-31560" windowWidth="25600" windowHeight="31560" activeTab="1" xr2:uid="{F4EE8929-4E87-DE4C-8476-CAC14DB8317E}"/>
+    <workbookView minimized="1" xWindow="-5080" yWindow="-31560" windowWidth="14460" windowHeight="20040" activeTab="2" xr2:uid="{F4EE8929-4E87-DE4C-8476-CAC14DB8317E}"/>
   </bookViews>
   <sheets>
     <sheet name="iPad version" sheetId="1" r:id="rId1"/>
     <sheet name="proto1" sheetId="2" r:id="rId2"/>
+    <sheet name="OSC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="177">
   <si>
     <t>Noisebox 2018 control variables</t>
   </si>
@@ -2837,8 +2838,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5199,4 +5200,678 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173FC7A0-3F3C-8240-8134-0B37E9006372}">
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT(B3,C3,"/",D3," - ")</f>
+        <v xml:space="preserve">/raspberrypi/0/0 - </v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F12" si="0">_xlfn.CONCAT(B4,C4,"/",D4," - ")</f>
+        <v xml:space="preserve">/raspberrypi/0/1 - </v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/2 - </v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/3 - </v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/4 - </v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/5 - </v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/6 - </v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">/raspberrypi/0/7 - </v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <f>_xlfn.CONCAT(B12,C12,"/",D12," - ", A12)</f>
+        <v>/raspberrypi/1/0 - button1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F19" si="1">_xlfn.CONCAT(B13,C13,"/",D13," - ", A13)</f>
+        <v>/raspberrypi/1/1 - button2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/2 - button3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/3 - button4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/4 - knob1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/5 - knob2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>6</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/6 - knob3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>7</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>/raspberrypi/1/7 - knob4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="5">
+        <v>10</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="5">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="5">
+        <v>10</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" s="5">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="5">
+        <v>10</v>
+      </c>
+      <c r="D28" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="5">
+        <v>10</v>
+      </c>
+      <c r="D29" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="5">
+        <v>10</v>
+      </c>
+      <c r="D30" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="5">
+        <v>11</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="5">
+        <v>11</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="5">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="5">
+        <v>11</v>
+      </c>
+      <c r="D34" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="5">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C36" s="5">
+        <v>11</v>
+      </c>
+      <c r="D36" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="5">
+        <v>11</v>
+      </c>
+      <c r="D37" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="5">
+        <v>11</v>
+      </c>
+      <c r="D38" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="5">
+        <v>11</v>
+      </c>
+      <c r="D39" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="5">
+        <v>11</v>
+      </c>
+      <c r="D40" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="35"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="5">
+        <v>12</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="5">
+        <v>12</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="5">
+        <v>12</v>
+      </c>
+      <c r="D44" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>